<commit_message>
new files were added
</commit_message>
<xml_diff>
--- a/atoka/atoka/spiders/input/input100.xlsx
+++ b/atoka/atoka/spiders/input/input100.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="103">
   <si>
     <t xml:space="preserve">01905300164</t>
   </si>
@@ -446,7 +446,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1048576"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -455,7 +455,7 @@
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.1"/>
@@ -476,572 +476,579 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" s="0"/>
       <c r="D3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="0"/>
       <c r="D4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" s="0"/>
       <c r="D5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C6" s="0"/>
       <c r="D6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" s="0"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C19" s="0"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
-        <v>19</v>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C21" s="0"/>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C38" s="0"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
-        <v>38</v>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C40" s="0"/>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
-        <v>40</v>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C43" s="0"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
-        <v>43</v>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="C44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C45" s="0"/>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
-        <v>45</v>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C47" s="0"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="2" t="s">
-        <v>47</v>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="C48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>57</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>80</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="3" t="s">
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="2" t="s">
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="2" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>